<commit_message>
Iniciando versao predicao Link
</commit_message>
<xml_diff>
--- a/PredLig/src/Documentation/Resultados/Results and Diferences_min-edges3-weighted-combLinear-1999-nowell.xlsx
+++ b/PredLig/src/Documentation/Resultados/Results and Diferences_min-edges3-weighted-combLinear-1999-nowell.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="14025" windowHeight="4425" activeTab="4"/>
@@ -11,14 +11,14 @@
     <sheet name="Results 1994-1999" sheetId="4" r:id="rId2"/>
     <sheet name="GR-QC" sheetId="9" r:id="rId3"/>
     <sheet name="HEP-TH" sheetId="10" r:id="rId4"/>
-    <sheet name="HEP-PH" sheetId="11" r:id="rId5"/>
-    <sheet name="COND-MAT" sheetId="12" r:id="rId6"/>
+    <sheet name="COND-MAT" sheetId="12" r:id="rId5"/>
+    <sheet name="HEP-PH" sheetId="11" r:id="rId6"/>
     <sheet name="ASTRO-PH" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -157,11 +157,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +387,8 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,12 +410,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -455,17 +455,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -489,41 +480,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -579,7 +549,7 @@
             <c:numRef>
               <c:f>'Results 1994-1999'!$D$7:$D$33</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>27.8673</c:v>
@@ -627,61 +597,44 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="531287552"/>
-        <c:axId val="531226624"/>
+        <c:axId val="81523456"/>
+        <c:axId val="81524992"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="531287552"/>
+        <c:axId val="81523456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531226624"/>
+        <c:crossAx val="81524992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531226624"/>
+        <c:axId val="81524992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531287552"/>
+        <c:crossAx val="81523456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -689,17 +642,8 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -723,41 +667,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -813,7 +736,7 @@
             <c:numRef>
               <c:f>'Results 1994-1999'!$E$7:$E$33</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>42.69071526578886</c:v>
@@ -855,67 +778,50 @@
                   <c:v>52.223593431935896</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>38.960458592079156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="536332288"/>
-        <c:axId val="538882560"/>
+        <c:axId val="81808000"/>
+        <c:axId val="81846656"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="536332288"/>
+        <c:axId val="81808000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538882560"/>
+        <c:crossAx val="81846656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="538882560"/>
+        <c:axId val="81846656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536332288"/>
+        <c:crossAx val="81808000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -923,251 +829,8 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>HEP-PH</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> - Random = 0,21</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>Common Neighbors</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Adamic Adar similarity</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Jaccard similarity coefficient</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Preferential Attachment</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Time Score DF 0.2 </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Time Score DF 0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Time Score DF 0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>cnW Time Score DF 0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>cnW Time Score DF 0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>cnW Time Score DF 0.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>aaW Time Score DF 0.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>aaW Time Score DF 0.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>aaW Time Score DF 0.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Combinacao Linear (cn, aas, jc, pa, ts08, ts05, ts02)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Results 1994-1999'!$F$7:$F$33</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>25.863677367434825</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28.802731613734235</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>28.655778901419264</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.842223943812028</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26.598440929009676</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26.451488216694706</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>26.451488216694706</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>26.451488216694706</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>26.304535504379736</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>27.186251778269558</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>31.153975010773763</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31.447880435403704</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>31.594833147718681</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="cylinder"/>
-        <c:axId val="536734720"/>
-        <c:axId val="571963584"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="536734720"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571963584"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="571963584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536734720"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1191,41 +854,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1281,7 +923,7 @@
             <c:numRef>
               <c:f>'Results 1994-1999'!$G$7:$G$33</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43.19165746691872</c:v>
@@ -1323,67 +965,236 @@
                   <c:v>52.658322117202268</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>52.658322117202268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="536732672"/>
-        <c:axId val="571961856"/>
+        <c:axId val="82348672"/>
+        <c:axId val="82350464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="536732672"/>
+        <c:axId val="82348672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571961856"/>
+        <c:crossAx val="82350464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571961856"/>
+        <c:axId val="82350464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536732672"/>
+        <c:crossAx val="82348672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:style val="3"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>HEP-PH</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> - Random = 0,21</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Common Neighbors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Adamic Adar similarity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jaccard similarity coefficient</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Preferential Attachment</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Time Score DF 0.2 </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Time Score DF 0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Time Score DF 0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cnW Time Score DF 0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>cnW Time Score DF 0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>cnW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>aaW Time Score DF 0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>aaW Time Score DF 0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear (cn, aas, jc, pa, ts08, ts05, ts02)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Results 1994-1999'!$F$7:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>25.863677367434825</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.802731613734235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.655778901419264</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.842223943812028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.598440929009676</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.451488216694706</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.451488216694706</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.451488216694706</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.304535504379736</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.186251778269558</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.153975010773763</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.447880435403704</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.594833147718681</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:shape val="cylinder"/>
+        <c:axId val="82047744"/>
+        <c:axId val="82049280"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="82047744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82049280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82049280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82047744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1391,17 +1202,8 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1424,42 +1226,20 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1515,7 +1295,7 @@
             <c:numRef>
               <c:f>'Results 1994-1999'!$H$7:$H$33</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>18.569897666750389</c:v>
@@ -1563,61 +1343,44 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="538472448"/>
-        <c:axId val="572428800"/>
+        <c:axId val="82420096"/>
+        <c:axId val="82421632"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="538472448"/>
+        <c:axId val="82420096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="572428800"/>
+        <c:crossAx val="82421632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572428800"/>
+        <c:axId val="82421632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538472448"/>
+        <c:crossAx val="82420096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1699,15 +1462,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1736,15 +1499,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1807,9 +1570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1847,7 +1610,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1881,7 +1644,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1916,10 +1678,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2092,14 +1853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
@@ -2108,20 +1869,20 @@
     <col min="19" max="19" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:12" ht="32.25" customHeight="1">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
@@ -2144,7 +1905,7 @@
       </c>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2168,7 +1929,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -2192,7 +1953,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -2216,7 +1977,7 @@
         <v>3294</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -2240,7 +2001,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -2264,7 +2025,7 @@
         <v>5751</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2274,19 +2035,19 @@
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="2:12" ht="36" customHeight="1">
+      <c r="B10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="29"/>
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
@@ -2308,7 +2069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2332,7 +2093,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2356,7 +2117,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
@@ -2380,7 +2141,7 @@
         <v>3294</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -2404,7 +2165,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
@@ -2428,7 +2189,7 @@
         <v>5751</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2438,19 +2199,19 @@
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
+    <row r="18" spans="1:12" ht="24.75" customHeight="1">
+      <c r="B18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
@@ -2473,7 +2234,7 @@
       </c>
       <c r="L19" s="11"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
@@ -2483,7 +2244,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2513,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="16"/>
       <c r="B22" s="12" t="s">
         <v>6</v>
@@ -2545,7 +2306,7 @@
       </c>
       <c r="J22" s="16"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="B23" s="8" t="s">
         <v>7</v>
       </c>
@@ -2575,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="B24" s="12" t="s">
         <v>8</v>
       </c>
@@ -2605,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
       <c r="B25" s="5" t="s">
         <v>9</v>
       </c>
@@ -2647,14 +2408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="3" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -2663,23 +2424,23 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="29">
+    <row r="1" spans="3:8">
+      <c r="C1" s="22">
         <f>((G26/ 'First Table'!I15  )*100)/G5</f>
         <v>51.474989035916821</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="28" t="s">
+    <row r="2" spans="3:8">
+      <c r="C2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+    </row>
+    <row r="4" spans="3:8">
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2699,7 +2460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8">
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2724,7 +2485,7 @@
         <v>0.47473918649630759</v>
       </c>
     </row>
-    <row r="6" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2744,7 +2505,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="7" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" collapsed="1">
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2769,7 +2530,7 @@
         <v>18.569897666750389</v>
       </c>
     </row>
-    <row r="8" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2789,7 +2550,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="9" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" collapsed="1">
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
@@ -2814,7 +2575,7 @@
         <v>20.254740453082768</v>
       </c>
     </row>
-    <row r="10" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
@@ -2834,7 +2595,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" collapsed="1">
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2620,7 @@
         <v>16.592038743664546</v>
       </c>
     </row>
-    <row r="12" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2879,7 +2640,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" collapsed="1">
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2904,7 +2665,7 @@
         <v>4.7615122222436899</v>
       </c>
     </row>
-    <row r="14" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2924,7 +2685,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="15" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" collapsed="1">
       <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2949,7 +2710,7 @@
         <v>17.764103290678378</v>
       </c>
     </row>
-    <row r="16" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
@@ -2969,7 +2730,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="17" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" collapsed="1">
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2994,7 +2755,7 @@
         <v>17.617595222301649</v>
       </c>
     </row>
-    <row r="18" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" hidden="1" outlineLevel="2">
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
@@ -3014,7 +2775,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="19" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" collapsed="1">
       <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
@@ -3039,8 +2800,8 @@
         <v>17.434460136830737</v>
       </c>
     </row>
-    <row r="20" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C20" s="30" t="s">
+    <row r="20" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C20" s="23" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="1">
@@ -3059,8 +2820,8 @@
         <v>429</v>
       </c>
     </row>
-    <row r="21" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="30" t="s">
+    <row r="21" spans="3:8" collapsed="1">
+      <c r="C21" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="20">
@@ -3084,8 +2845,8 @@
         <v>15.712990333404173</v>
       </c>
     </row>
-    <row r="22" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C22" s="30" t="s">
+    <row r="22" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C22" s="23" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="1">
@@ -3104,8 +2865,8 @@
         <v>430</v>
       </c>
     </row>
-    <row r="23" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="30" t="s">
+    <row r="23" spans="3:8" collapsed="1">
+      <c r="C23" s="23" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="20">
@@ -3129,8 +2890,8 @@
         <v>15.749617350498356</v>
       </c>
     </row>
-    <row r="24" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C24" s="30" t="s">
+    <row r="24" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C24" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="1">
@@ -3149,8 +2910,8 @@
         <v>458</v>
       </c>
     </row>
-    <row r="25" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="30" t="s">
+    <row r="25" spans="3:8" collapsed="1">
+      <c r="C25" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="20">
@@ -3174,8 +2935,8 @@
         <v>16.775173829135458</v>
       </c>
     </row>
-    <row r="26" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C26" s="30" t="s">
+    <row r="26" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C26" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="1">
@@ -3194,8 +2955,8 @@
         <v>491</v>
       </c>
     </row>
-    <row r="27" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="30" t="s">
+    <row r="27" spans="3:8" collapsed="1">
+      <c r="C27" s="23" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="20">
@@ -3219,8 +2980,8 @@
         <v>17.983865393243473</v>
       </c>
     </row>
-    <row r="28" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C28" s="30" t="s">
+    <row r="28" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C28" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="1">
@@ -3239,8 +3000,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="30" t="s">
+    <row r="29" spans="3:8" collapsed="1">
+      <c r="C29" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="20">
@@ -3264,8 +3025,8 @@
         <v>18.606524683844572</v>
       </c>
     </row>
-    <row r="30" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C30" s="30" t="s">
+    <row r="30" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C30" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="1">
@@ -3284,8 +3045,8 @@
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="30" t="s">
+    <row r="31" spans="3:8" collapsed="1">
+      <c r="C31" s="23" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="20">
@@ -3309,20 +3070,24 @@
         <v>18.569897666750389</v>
       </c>
     </row>
-    <row r="32" spans="3:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C32" s="30" t="s">
+    <row r="32" spans="3:8" hidden="1" outlineLevel="2">
+      <c r="C32" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="1">
         <v>32</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>94</v>
+      </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1">
+        <v>89</v>
+      </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="3:8" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="30" t="s">
+    <row r="33" spans="3:8" collapsed="1">
+      <c r="C33" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="20">
@@ -3331,7 +3096,7 @@
       </c>
       <c r="E33" s="20">
         <f>((E32/   'First Table'!I13   )*100)/E5</f>
-        <v>0</v>
+        <v>38.960458592079156</v>
       </c>
       <c r="F33" s="20">
         <f>((F32/   'First Table'!I14    )*100)/F5</f>
@@ -3339,7 +3104,7 @@
       </c>
       <c r="G33" s="20">
         <f>((G32/ 'First Table'!I15  )*100)/G5</f>
-        <v>0</v>
+        <v>52.658322117202268</v>
       </c>
       <c r="H33" s="20">
         <f>((H32/   'First Table'!I16    )*100)/H5</f>
@@ -3356,14 +3121,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3371,14 +3136,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -3386,47 +3151,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" ht="12" customHeight="1"/>
+    <row r="2" ht="12.75" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Subindo versao com o resultado do primeiro AG.
</commit_message>
<xml_diff>
--- a/PredLig/src/Documentation/Resultados/Results and Diferences_min-edges3-weighted-combLinear-1999-nowell.xlsx
+++ b/PredLig/src/Documentation/Resultados/Results and Diferences_min-edges3-weighted-combLinear-1999-nowell.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="First Table" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Article Data</t>
   </si>
@@ -151,7 +151,10 @@
     <t>aaW Time Score DF 0.2</t>
   </si>
   <si>
-    <t>Combinacao Linear (cn, aas, jc, pa, ts08, ts05, ts02)</t>
+    <t>Combinacao Linear</t>
+  </si>
+  <si>
+    <t>Combinacao Linear (Total Success)</t>
   </si>
 </sst>
 </file>
@@ -351,15 +354,6 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -383,6 +377,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -541,7 +544,7 @@
             <c:strRef>
               <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Common Neighbors</c:v>
                 </c:pt>
@@ -580,6 +583,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -589,7 +595,7 @@
               <c:f>'Results 1994-1999'!$D$7:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>27.8673</c:v>
                 </c:pt>
@@ -628,18 +634,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.600650000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.73385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="103028608"/>
-        <c:axId val="103030144"/>
+        <c:axId val="85731200"/>
+        <c:axId val="85732736"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="103028608"/>
+        <c:axId val="85731200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,14 +678,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103030144"/>
+        <c:crossAx val="85732736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103030144"/>
+        <c:axId val="85732736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,7 +725,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103028608"/>
+        <c:crossAx val="85731200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -743,7 +752,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -829,7 +838,7 @@
             <c:strRef>
               <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Common Neighbors</c:v>
                 </c:pt>
@@ -868,6 +877,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -877,7 +889,7 @@
               <c:f>'Results 1994-1999'!$E$7:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>42.69071526578886</c:v>
                 </c:pt>
@@ -916,18 +928,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>52.223593431935896</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49.736755649462758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="103084032"/>
-        <c:axId val="103085568"/>
+        <c:axId val="85782528"/>
+        <c:axId val="85784064"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="103084032"/>
+        <c:axId val="85782528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,14 +972,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103085568"/>
+        <c:crossAx val="85784064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103085568"/>
+        <c:axId val="85784064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,7 +1019,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103084032"/>
+        <c:crossAx val="85782528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1031,7 +1046,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1117,7 +1132,7 @@
             <c:strRef>
               <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Common Neighbors</c:v>
                 </c:pt>
@@ -1156,6 +1171,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1165,7 +1183,7 @@
               <c:f>'Results 1994-1999'!$F$7:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>25.863677367434825</c:v>
                 </c:pt>
@@ -1204,18 +1222,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>31.594833147718681</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.039299065954587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="113239936"/>
-        <c:axId val="113241472"/>
+        <c:axId val="85792640"/>
+        <c:axId val="85794176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113239936"/>
+        <c:axId val="85792640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,14 +1266,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113241472"/>
+        <c:crossAx val="85794176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113241472"/>
+        <c:axId val="85794176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1313,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113239936"/>
+        <c:crossAx val="85792640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1319,7 +1340,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1405,7 +1426,7 @@
             <c:strRef>
               <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Common Neighbors</c:v>
                 </c:pt>
@@ -1444,6 +1465,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1453,7 +1477,7 @@
               <c:f>'Results 1994-1999'!$G$7:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43.19165746691872</c:v>
                 </c:pt>
@@ -1492,18 +1516,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>52.658322117202268</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.616654820415874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="113295360"/>
-        <c:axId val="113296896"/>
+        <c:axId val="86114304"/>
+        <c:axId val="86115840"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113295360"/>
+        <c:axId val="86114304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,14 +1560,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113296896"/>
+        <c:crossAx val="86115840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113296896"/>
+        <c:axId val="86115840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1607,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113295360"/>
+        <c:crossAx val="86114304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,7 +1634,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1693,7 +1720,7 @@
             <c:strRef>
               <c:f>'Results 1994-1999'!$C$7:$C$33</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Common Neighbors</c:v>
                 </c:pt>
@@ -1732,6 +1759,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>aaW Time Score DF 0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Combinacao Linear</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1741,7 +1771,7 @@
               <c:f>'Results 1994-1999'!$H$7:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>18.569897666750389</c:v>
                 </c:pt>
@@ -1780,18 +1810,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>18.569897666750389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.181486418894405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="113374720"/>
-        <c:axId val="113376256"/>
+        <c:axId val="86513152"/>
+        <c:axId val="86514688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="113374720"/>
+        <c:axId val="86513152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,14 +1854,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113376256"/>
+        <c:crossAx val="86514688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113376256"/>
+        <c:axId val="86514688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1901,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113374720"/>
+        <c:crossAx val="86513152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1895,7 +1928,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1953,7 +1986,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2363,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2381,527 +2414,527 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="32.25" customHeight="1">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>2122</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>3287</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>5724</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>486</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>519</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="7">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>5241</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>9498</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="2">
         <v>15842</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>1438</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="2">
         <v>2311</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>1576</v>
       </c>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>5414</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>10254</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <v>47806</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <v>1790</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="2">
         <v>6654</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>3294</v>
       </c>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>5469</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>6700</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <v>19881</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>1253</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>1899</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>1150</v>
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>5343</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>5816</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <v>41852</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>1561</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="2">
         <v>6178</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>5751</v>
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="10"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:12" ht="36" customHeight="1">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>2122</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <v>3287</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <v>5722</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="2">
         <v>486</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="2">
         <v>519</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>400</v>
       </c>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>5241</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <v>9498</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <v>15834</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="2">
         <v>1437</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="2">
         <v>2308</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <v>1576</v>
       </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>5414</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="2">
         <v>10254</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="2">
         <v>47800</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="2">
         <v>1790</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="2">
         <v>6654</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="7">
         <v>3294</v>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>5469</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="2">
         <v>6700</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="2">
         <v>19878</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="2">
         <v>1253</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="2">
         <v>1899</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>1150</v>
       </c>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <v>5343</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="2">
         <v>5816</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="2">
         <v>41848</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="2">
         <v>1561</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="2">
         <v>6178</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="7">
         <v>5751</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="10"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:12" ht="24.75" customHeight="1">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="11"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
         <f t="shared" ref="D21:I25" si="0">D4-D12</f>
         <v>0</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15">
+      <c r="C22" s="11"/>
+      <c r="D22" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="12"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="5">
+      <c r="C23" s="15"/>
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15">
+      <c r="C24" s="11"/>
+      <c r="D24" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="5">
+      <c r="C25" s="16"/>
+      <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2922,7 +2955,7 @@
   <dimension ref="C1:H33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2"/>
@@ -2938,681 +2971,691 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:8">
-      <c r="C1" s="20"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="3:8">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="4" spans="3:8">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:8">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <f>( 'First Table'!I12 / ( ( ('First Table'!G12 * ('First Table'!G12 - 1))/2) - 'First Table'!H12) *100)</f>
         <v>0.340901343151292</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <f>( 'First Table'!I13 / ( ( ('First Table'!G13 * ('First Table'!G13 - 1))/2) - 'First Table'!H13)*100)</f>
         <v>0.15309026691715447</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <f>( 'First Table'!I14 / ( ( ('First Table'!G14 * ('First Table'!G14 - 1))/2) - 'First Table'!H14)*100)</f>
         <v>0.20658500684540176</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <f>( 'First Table'!I15 / ( ( ('First Table'!G15 * ('First Table'!G15 - 1))/2) - 'First Table'!H15)*100 )</f>
         <v>0.1469688004406508</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="19">
         <f>( 'First Table'!I16 / ( ( ('First Table'!G16 * ('First Table'!G16 - 1))/2) - 'First Table'!H16) *100)</f>
         <v>0.47473918649630759</v>
       </c>
     </row>
     <row r="6" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>38</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>103</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>176</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>73</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>507</v>
       </c>
     </row>
     <row r="7" spans="3:8" collapsed="1">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <f>((D6/ 'First Table'!I12  )*100)/D5</f>
         <v>27.8673</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <f>((E6/   'First Table'!I13    )*100)/E5</f>
         <v>42.69071526578886</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <f>((F6/   'First Table'!I14    )*100)/F5</f>
         <v>25.863677367434825</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <f>((G6/   'First Table'!I15    )*100)/G5</f>
         <v>43.19165746691872</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <f>((H6/   'First Table'!I16    )*100)/H5</f>
         <v>18.569897666750389</v>
       </c>
     </row>
     <row r="8" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>31</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>117</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>196</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>74</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <v>553</v>
       </c>
     </row>
     <row r="9" spans="3:8" collapsed="1">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <f>((D8/ 'First Table'!I12  )*100)/D5</f>
         <v>22.73385</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <f>((E8/   'First Table'!I13    )*100)/E5</f>
         <v>48.493336758226185</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <f>((F8/   'First Table'!I14    )*100)/F5</f>
         <v>28.802731613734235</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="22">
         <f>((G8/ 'First Table'!I15  )*100)/G5</f>
         <v>43.78332400756144</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <f>((H8/   'First Table'!I16    )*100)/H5</f>
         <v>20.254740453082768</v>
       </c>
     </row>
     <row r="10" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>29</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>111</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <v>195</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <v>75</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>453</v>
       </c>
     </row>
     <row r="11" spans="3:8" collapsed="1">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <f>((D10/ 'First Table'!I12  )*100)/D5</f>
         <v>21.267149999999997</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="22">
         <f>((E10/   'First Table'!I13    )*100)/E5</f>
         <v>46.006498975753047</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="22">
         <f>((F10/   'First Table'!I14    )*100)/F5</f>
         <v>28.655778901419264</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="22">
         <f>((G10/ 'First Table'!I15  )*100)/G5</f>
         <v>44.374990548204153</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="21">
         <f>((H10/   'First Table'!I16    )*100)/H5</f>
         <v>16.592038743664546</v>
       </c>
     </row>
     <row r="12" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <v>8</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>19</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <v>101</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <v>9</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="21">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="3:8" collapsed="1">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="21">
         <f>((D12/ 'First Table'!I12  )*100)/D5</f>
         <v>5.8668000000000005</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <f>((E12/   'First Table'!I13    )*100)/E5</f>
         <v>7.8749863111649363</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <f>((F12/   'First Table'!I14    )*100)/F5</f>
         <v>14.842223943812028</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <f>((G12/ 'First Table'!I15  )*100)/G5</f>
         <v>5.3249988657844991</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="21">
         <f>((H12/   'First Table'!I16    )*100)/H5</f>
         <v>4.7615122222436899</v>
       </c>
     </row>
     <row r="14" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
         <v>39</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>119</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>181</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>87</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="21">
         <v>485</v>
       </c>
     </row>
     <row r="15" spans="3:8" collapsed="1">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <f>((D14/ 'First Table'!I12  )*100)/D5</f>
         <v>28.600650000000002</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <f>((E14/   'First Table'!I13   )*100)/E5</f>
         <v>49.322282685717234</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <f>((F14/   'First Table'!I14    )*100)/F5</f>
         <v>26.598440929009676</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <f>((G14/ 'First Table'!I15  )*100)/G5</f>
         <v>51.474989035916821</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="21">
         <f>((H14/   'First Table'!I16    )*100)/H5</f>
         <v>17.764103290678378</v>
       </c>
     </row>
     <row r="16" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>44</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>117</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="21">
         <v>180</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <v>86</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="21">
         <v>481</v>
       </c>
     </row>
     <row r="17" spans="3:8" collapsed="1">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <f>((D16/ 'First Table'!I12  )*100)/D5</f>
         <v>32.267400000000002</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <f>((E16/   'First Table'!I13   )*100)/E5</f>
         <v>48.493336758226185</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="21">
         <f>((F16/   'First Table'!I14    )*100)/F5</f>
         <v>26.451488216694706</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="21">
         <f>((G16/ 'First Table'!I15  )*100)/G5</f>
         <v>50.883322495274108</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="21">
         <f>((H16/   'First Table'!I16    )*100)/H5</f>
         <v>17.617595222301649</v>
       </c>
     </row>
     <row r="18" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>43</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>111</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="21">
         <v>180</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="21">
         <v>87</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="21">
         <v>476</v>
       </c>
     </row>
     <row r="19" spans="3:8" collapsed="1">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <f>((D18/ 'First Table'!I12  )*100)/D5</f>
         <v>31.534050000000001</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <f>((E18/   'First Table'!I13   )*100)/E5</f>
         <v>46.006498975753047</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="21">
         <f>((F18/   'First Table'!I14    )*100)/F5</f>
         <v>26.451488216694706</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="21">
         <f>((G18/ 'First Table'!I15  )*100)/G5</f>
         <v>51.474989035916821</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="21">
         <f>((H18/   'First Table'!I16    )*100)/H5</f>
         <v>17.434460136830737</v>
       </c>
     </row>
     <row r="20" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="2">
         <v>39</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="2">
         <v>110</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="2">
         <v>180</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="2">
         <v>86</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="2">
         <v>429</v>
       </c>
     </row>
     <row r="21" spans="3:8" collapsed="1">
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <f>((D20/ 'First Table'!I12  )*100)/D5</f>
         <v>28.600650000000002</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="21">
         <f>((E20/   'First Table'!I13   )*100)/E5</f>
         <v>45.592026012007523</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="21">
         <f>((F20/   'First Table'!I14    )*100)/F5</f>
         <v>26.451488216694706</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="21">
         <f>((G20/ 'First Table'!I15  )*100)/G5</f>
         <v>50.883322495274108</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="21">
         <f>((H20/   'First Table'!I16    )*100)/H5</f>
         <v>15.712990333404173</v>
       </c>
     </row>
     <row r="22" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="2">
         <v>40</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="2">
         <v>114</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="2">
         <v>179</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="2">
         <v>89</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="2">
         <v>430</v>
       </c>
     </row>
     <row r="23" spans="3:8" collapsed="1">
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <f>((D22/ 'First Table'!I12  )*100)/D5</f>
         <v>29.334</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <f>((E22/   'First Table'!I13   )*100)/E5</f>
         <v>47.249917866989612</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="21">
         <f>((F22/   'First Table'!I14    )*100)/F5</f>
         <v>26.304535504379736</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="21">
         <f>((G22/ 'First Table'!I15  )*100)/G5</f>
         <v>52.658322117202268</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="21">
         <f>((H22/   'First Table'!I16    )*100)/H5</f>
         <v>15.749617350498356</v>
       </c>
     </row>
     <row r="24" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="2">
         <v>40</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="2">
         <v>119</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="2">
         <v>185</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="2">
         <v>89</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="2">
         <v>458</v>
       </c>
     </row>
     <row r="25" spans="3:8" collapsed="1">
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="21">
         <f>((D24/ 'First Table'!I12  )*100)/D5</f>
         <v>29.334</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <f>((E24/   'First Table'!I13   )*100)/E5</f>
         <v>49.322282685717234</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="21">
         <f>((F24/   'First Table'!I14    )*100)/F5</f>
         <v>27.186251778269558</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="21">
         <f>((G24/ 'First Table'!I15  )*100)/G5</f>
         <v>52.658322117202268</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="21">
         <f>((H24/   'First Table'!I16    )*100)/H5</f>
         <v>16.775173829135458</v>
       </c>
     </row>
     <row r="26" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="2">
         <v>34</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="2">
         <v>116</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="2">
         <v>212</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="2">
         <v>87</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="2">
         <v>491</v>
       </c>
     </row>
     <row r="27" spans="3:8" collapsed="1">
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <f>((D26/ 'First Table'!I12  )*100)/D5</f>
         <v>24.933900000000001</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <f>((E26/   'First Table'!I13   )*100)/E5</f>
         <v>48.078863794480661</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="21">
         <f>((F26/   'First Table'!I14    )*100)/F5</f>
         <v>31.153975010773763</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="21">
         <f>((G26/ 'First Table'!I15  )*100)/G5</f>
         <v>51.474989035916821</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="21">
         <f>((H26/   'First Table'!I16    )*100)/H5</f>
         <v>17.983865393243473</v>
       </c>
     </row>
     <row r="28" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="2">
         <v>38</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="2">
         <v>126</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="2">
         <v>214</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="2">
         <v>91</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="2">
         <v>508</v>
       </c>
     </row>
     <row r="29" spans="3:8" collapsed="1">
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <f>((D28/ 'First Table'!I12  )*100)/D5</f>
         <v>27.8673</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="21">
         <f>((E28/   'First Table'!I13   )*100)/E5</f>
         <v>52.223593431935896</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="21">
         <f>((F28/   'First Table'!I14    )*100)/F5</f>
         <v>31.447880435403704</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="21">
         <f>((G28/ 'First Table'!I15  )*100)/G5</f>
         <v>53.841655198487715</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="21">
         <f>((H28/   'First Table'!I16    )*100)/H5</f>
         <v>18.606524683844572</v>
       </c>
     </row>
     <row r="30" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="2">
         <v>39</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="2">
         <v>126</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="2">
         <v>215</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="2">
         <v>89</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="2">
         <v>507</v>
       </c>
     </row>
     <row r="31" spans="3:8" collapsed="1">
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="21">
         <f>((D30/ 'First Table'!I12  )*100)/D5</f>
         <v>28.600650000000002</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="21">
         <f>((E30/   'First Table'!I13   )*100)/E5</f>
         <v>52.223593431935896</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="21">
         <f>((F30/   'First Table'!I14    )*100)/F5</f>
         <v>31.594833147718681</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="21">
         <f>((G30/ 'First Table'!I15  )*100)/G5</f>
         <v>52.658322117202268</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H31" s="21">
         <f>((H30/   'First Table'!I16    )*100)/H5</f>
         <v>18.569897666750389</v>
       </c>
     </row>
     <row r="32" spans="3:8" hidden="1" outlineLevel="2">
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="2">
+        <v>31</v>
+      </c>
+      <c r="E32" s="2">
+        <v>120</v>
+      </c>
+      <c r="F32" s="2">
+        <v>184</v>
+      </c>
+      <c r="G32" s="2">
+        <v>94</v>
+      </c>
+      <c r="H32" s="2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" collapsed="1">
+      <c r="C33" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="3:8" hidden="1" collapsed="1">
-      <c r="C33" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="24">
+      <c r="D33" s="21">
         <f>((D32/ 'First Table'!I12  )*100)/D5</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="24">
+        <v>22.73385</v>
+      </c>
+      <c r="E33" s="21">
         <f>((E32/   'First Table'!I13   )*100)/E5</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="24">
+        <v>49.736755649462758</v>
+      </c>
+      <c r="F33" s="21">
         <f>((F32/   'First Table'!I14    )*100)/F5</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="24">
+        <v>27.039299065954587</v>
+      </c>
+      <c r="G33" s="21">
         <f>((G32/ 'First Table'!I15  )*100)/G5</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="24">
+        <v>55.616654820415874</v>
+      </c>
+      <c r="H33" s="21">
         <f>((H32/   'First Table'!I16    )*100)/H5</f>
-        <v>0</v>
+        <v>20.181486418894405</v>
       </c>
     </row>
   </sheetData>
@@ -3707,7 +3750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>